<commit_message>
versión revisada posterior a defensa de tfm
</commit_message>
<xml_diff>
--- a/CouriersCR/notebooks/forecast.xlsx
+++ b/CouriersCR/notebooks/forecast.xlsx
@@ -487,10 +487,10 @@
         <v>5408.531617848117</v>
       </c>
       <c r="C2" t="n">
-        <v>-4550.348811941487</v>
+        <v>-4976.313244358554</v>
       </c>
       <c r="D2" t="n">
-        <v>15828.67946564393</v>
+        <v>16209.14789398284</v>
       </c>
       <c r="E2" t="n">
         <v>13992.81761010253</v>
@@ -513,10 +513,10 @@
         <v>11028.7923459348</v>
       </c>
       <c r="C3" t="n">
-        <v>432.2100096499077</v>
+        <v>636.2068445654998</v>
       </c>
       <c r="D3" t="n">
-        <v>21098.12235703578</v>
+        <v>21164.59471585847</v>
       </c>
       <c r="E3" t="n">
         <v>13997.5031538284</v>
@@ -539,10 +539,10 @@
         <v>23015.24077949795</v>
       </c>
       <c r="C4" t="n">
-        <v>12859.54792092447</v>
+        <v>11947.94006750283</v>
       </c>
       <c r="D4" t="n">
-        <v>33669.79255935108</v>
+        <v>33657.12323262377</v>
       </c>
       <c r="E4" t="n">
         <v>14002.18869755426</v>
@@ -565,10 +565,10 @@
         <v>13026.89535343574</v>
       </c>
       <c r="C5" t="n">
-        <v>2875.576292711549</v>
+        <v>2130.00157561662</v>
       </c>
       <c r="D5" t="n">
-        <v>23232.4718832864</v>
+        <v>23817.13369383052</v>
       </c>
       <c r="E5" t="n">
         <v>14006.87424128012</v>
@@ -591,10 +591,10 @@
         <v>13384.09707091759</v>
       </c>
       <c r="C6" t="n">
-        <v>2826.167898678858</v>
+        <v>3452.861499942476</v>
       </c>
       <c r="D6" t="n">
-        <v>24336.48707112251</v>
+        <v>23777.46398335794</v>
       </c>
       <c r="E6" t="n">
         <v>14011.55978500599</v>

</xml_diff>